<commit_message>
Finish script 4 with Lukas' help, return new data
</commit_message>
<xml_diff>
--- a/Raw Data/Loggerdaten_2019_JJA/Standorte_2019_DEF.xlsx
+++ b/Raw Data/Loggerdaten_2019_JJA/Standorte_2019_DEF.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Masterarbeit\Masterarbeit_data\Daten 22.02.19\Temp_2018_data_cleared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\RIG-HeatMap\Raw Data\Loggerdaten_2019_JJA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C41661B-8CE1-47D0-9B65-87AF9AE9838D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24135" windowHeight="12285" tabRatio="230"/>
+    <workbookView xWindow="1155" yWindow="4350" windowWidth="25080" windowHeight="16065" tabRatio="230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -812,7 +813,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -992,6 +993,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1027,6 +1045,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1202,14 +1237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1304,7 +1339,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1342,7 +1377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1378,7 +1413,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -1414,7 +1449,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>9</v>
       </c>
@@ -1470,7 +1505,7 @@
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>10</v>
       </c>
@@ -1506,7 +1541,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>12</v>
       </c>
@@ -1542,7 +1577,7 @@
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>13</v>
       </c>
@@ -1578,7 +1613,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>14</v>
       </c>
@@ -1614,7 +1649,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>15</v>
       </c>
@@ -1650,7 +1685,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>17</v>
       </c>
@@ -1688,7 +1723,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>18</v>
       </c>
@@ -1724,7 +1759,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>19</v>
       </c>
@@ -1762,7 +1797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>20</v>
       </c>
@@ -1798,7 +1833,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>21</v>
       </c>
@@ -1836,7 +1871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>22</v>
       </c>
@@ -1872,7 +1907,7 @@
       </c>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>23</v>
       </c>
@@ -1910,7 +1945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>25</v>
       </c>
@@ -1946,7 +1981,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>26</v>
       </c>
@@ -1984,7 +2019,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>27</v>
       </c>
@@ -2020,7 +2055,7 @@
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>28</v>
       </c>
@@ -2056,7 +2091,7 @@
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>31</v>
       </c>
@@ -2092,7 +2127,7 @@
       </c>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>32</v>
       </c>
@@ -2130,7 +2165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>33</v>
       </c>
@@ -2168,7 +2203,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>34</v>
       </c>
@@ -2204,7 +2239,7 @@
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>35</v>
       </c>
@@ -2242,7 +2277,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>36</v>
       </c>
@@ -2280,7 +2315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>37</v>
       </c>
@@ -2318,7 +2353,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>38</v>
       </c>
@@ -2354,7 +2389,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>39</v>
       </c>
@@ -2392,7 +2427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>40</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42</v>
       </c>
@@ -2502,7 +2537,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44</v>
       </c>
@@ -2540,7 +2575,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>45</v>
       </c>
@@ -2576,7 +2611,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>47</v>
       </c>
@@ -2614,7 +2649,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>48</v>
       </c>
@@ -2652,7 +2687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>49</v>
       </c>
@@ -2690,7 +2725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>50</v>
       </c>
@@ -2726,7 +2761,7 @@
       </c>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>51</v>
       </c>
@@ -2764,7 +2799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>52</v>
       </c>
@@ -2802,7 +2837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>53</v>
       </c>
@@ -2840,7 +2875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>55</v>
       </c>
@@ -2881,7 +2916,7 @@
         <v>60</v>
       </c>
       <c r="B45" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>105</v>

</xml_diff>